<commit_message>
Processes Discription last change
</commit_message>
<xml_diff>
--- a/Emad Branch/Processes Descriptions.xlsx
+++ b/Emad Branch/Processes Descriptions.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="29">
   <si>
     <t>Processes Descriptions</t>
   </si>
@@ -61,12 +61,6 @@
     <t>Log In</t>
   </si>
   <si>
-    <t>source</t>
-  </si>
-  <si>
-    <t>report</t>
-  </si>
-  <si>
     <t>Yes</t>
   </si>
   <si>
@@ -74,6 +68,39 @@
   </si>
   <si>
     <t>The librarian can lend members there requested books and can return books from members</t>
+  </si>
+  <si>
+    <t>Fine report</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The librarian can bring information about fines into a report </t>
+  </si>
+  <si>
+    <t>Issued books report</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The librarian can inquire about the books that had been issued </t>
+  </si>
+  <si>
+    <t>Damaged books report</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The librarian can inquire about the books that had been classified as damaged books and deleted </t>
+  </si>
+  <si>
+    <t>Available books</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The librarian can inquire about the books that is available to be issued </t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>Report</t>
   </si>
 </sst>
 </file>
@@ -100,6 +127,7 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <u/>
       <sz val="11"/>
       <color theme="1"/>
@@ -116,7 +144,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -174,17 +202,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -280,6 +297,30 @@
         <color auto="1"/>
       </left>
       <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
       <top/>
       <bottom style="medium">
         <color auto="1"/>
@@ -290,28 +331,31 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -616,22 +660,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:L19"/>
+  <dimension ref="A2:L27"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="10" max="10" width="18.375" customWidth="1"/>
+    <col min="10" max="10" width="25.25" customWidth="1"/>
     <col min="12" max="12" width="15.375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" s="11"/>
-      <c r="B3" s="12"/>
+    <row r="3" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A3" s="8"/>
+      <c r="B3" s="9"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -640,287 +684,445 @@
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="2" t="s">
+      <c r="K3" s="22"/>
+      <c r="L3" s="23" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" s="13"/>
-      <c r="B4" s="14"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="4"/>
+      <c r="A4" s="10"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="3"/>
     </row>
     <row r="5" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="K5" s="4"/>
+      <c r="L5" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K6" s="14"/>
+      <c r="L6" s="15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7" s="20"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="16"/>
+      <c r="L7" s="3"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K8" s="16"/>
+      <c r="L8" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A9" s="20"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="16"/>
+      <c r="L9" s="3"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A10" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K10" s="16"/>
+      <c r="L10" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A11" s="20"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="16"/>
+      <c r="L11" s="3"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A12" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K12" s="16"/>
+      <c r="L12" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A13" s="20"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="16"/>
+      <c r="L13" s="3"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A14" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K14" s="16"/>
+      <c r="L14" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A15" s="20"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="16"/>
+      <c r="L15" s="3"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A16" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K16" s="16"/>
+      <c r="L16" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="5" t="s">
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A17" s="20"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="16"/>
+      <c r="L17" s="3"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A18" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="K5" s="5"/>
-      <c r="L5" s="7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A6" s="13"/>
-      <c r="B6" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="K6" s="17"/>
-      <c r="L6" s="18" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A7" s="13"/>
-      <c r="B7" s="15"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="19"/>
-      <c r="L7" s="4"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A8" s="13"/>
-      <c r="B8" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="K8" s="19"/>
-      <c r="L8" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A9" s="13"/>
-      <c r="B9" s="15"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="19"/>
-      <c r="L9" s="4"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A10" s="13"/>
-      <c r="B10" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="K10" s="19"/>
-      <c r="L10" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A11" s="13"/>
-      <c r="B11" s="15"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="19"/>
-      <c r="L11" s="4"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A12" s="13"/>
-      <c r="B12" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="K12" s="19"/>
-      <c r="L12" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A13" s="13"/>
-      <c r="B13" s="15"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="19"/>
-      <c r="L13" s="4"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A14" s="13"/>
-      <c r="B14" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="K14" s="19"/>
-      <c r="L14" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A15" s="13"/>
-      <c r="B15" s="15"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="19"/>
-      <c r="L15" s="4"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A16" s="13"/>
-      <c r="B16" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3" t="s">
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K18" s="16"/>
+      <c r="L18" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A19" s="20"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="16"/>
+      <c r="L19" s="3"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A20" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20" s="2"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="11"/>
+      <c r="J20" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="K16" s="19"/>
-      <c r="L16" s="4" t="s">
+      <c r="K20" s="16"/>
+      <c r="L20" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A17" s="13"/>
-      <c r="B17" s="15"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="19"/>
-      <c r="L17" s="4"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A18" s="13"/>
-      <c r="B18" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="K18" s="19"/>
-      <c r="L18" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="8"/>
-      <c r="B19" s="16"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="9"/>
-      <c r="I19" s="9"/>
-      <c r="J19" s="9"/>
-      <c r="K19" s="20"/>
-      <c r="L19" s="10"/>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A21" s="20"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="11"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="16"/>
+      <c r="L21" s="3"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A22" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" s="2"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="11"/>
+      <c r="J22" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K22" s="16"/>
+      <c r="L22" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A23" s="20"/>
+      <c r="B23" s="12"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="11"/>
+      <c r="I23" s="11"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="16"/>
+      <c r="L23" s="3"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A24" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24" s="2"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="11"/>
+      <c r="J24" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K24" s="16"/>
+      <c r="L24" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A25" s="20"/>
+      <c r="B25" s="12"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="11"/>
+      <c r="I25" s="11"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="16"/>
+      <c r="L25" s="3"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A26" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="B26" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C26" s="2"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="11"/>
+      <c r="J26" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K26" s="16"/>
+      <c r="L26" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="21"/>
+      <c r="B27" s="13"/>
+      <c r="C27" s="17"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="7"/>
+      <c r="H27" s="7"/>
+      <c r="I27" s="7"/>
+      <c r="J27" s="17"/>
+      <c r="K27" s="18"/>
+      <c r="L27" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="110" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="80" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>